<commit_message>
update Roll Length Model
</commit_message>
<xml_diff>
--- a/Roll Length Model.xlsx
+++ b/Roll Length Model.xlsx
@@ -1,24 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Digital Transform Training\DTE_090622 copy\Files for exercises\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Practical_Python_For_Modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA8C9B0-E6A4-4D20-8D59-1BD524E4D954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6066F7-1C9D-4D28-B988-1474FF48D3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="25448" windowHeight="14445" xr2:uid="{4FDF0578-8281-4B11-9B5F-4602E6B37CDC}"/>
+    <workbookView xWindow="1680" yWindow="510" windowWidth="35617" windowHeight="14707" xr2:uid="{4FDF0578-8281-4B11-9B5F-4602E6B37CDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
     <sheet name="Raw Data" sheetId="2" r:id="rId2"/>
     <sheet name="XLStepsSettings" sheetId="3" state="veryHidden" r:id="rId3"/>
     <sheet name="ExcelSteps" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Settings_" sheetId="5" state="veryHidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="Caliper">Model!$I$7</definedName>
+    <definedName name="Diam_Core">Model!$I$6</definedName>
+    <definedName name="Diam_Roll">Model!$I$5</definedName>
+    <definedName name="Length_Roll">Model!$I$9</definedName>
+    <definedName name="Length_Unit">Model!$I$12</definedName>
+    <definedName name="m_used_per_day">Model!$I$16</definedName>
+    <definedName name="Model">Model!$I:$I</definedName>
+    <definedName name="n_People">Model!$I$13</definedName>
+    <definedName name="rate_line">Model!$I$20</definedName>
+    <definedName name="ScenarioName">Model!$I$2</definedName>
+    <definedName name="sq_usage">Model!$I$14</definedName>
+    <definedName name="t_run">Model!$I$21</definedName>
+  </definedNames>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,30 +68,6 @@
             <family val="2"/>
           </rPr>
           <t>Calculated from slope on Raw Data worksheet</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{B46F72A4-327E-4A3B-A1BA-07286B8AA1B7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Calculated from experimental data on Raw Data worksheet</t>
         </r>
         <r>
           <rPr>
@@ -253,7 +244,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="86">
   <si>
     <t>Grp</t>
   </si>
@@ -515,7 +506,46 @@
     <t>Cushiony_TP</t>
   </si>
   <si>
-    <t>=PI()*(Diam_Roll^2 - Diam_Core^2)/(4*Caliper)/mm.m</t>
+    <t>Industrial Consumption</t>
+  </si>
+  <si>
+    <t>Line Speed</t>
+  </si>
+  <si>
+    <t>rate_line</t>
+  </si>
+  <si>
+    <t>m.min</t>
+  </si>
+  <si>
+    <t>Run Time</t>
+  </si>
+  <si>
+    <t>t_run</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>=ROUND(Length_Roll/rate_line,2)</t>
+  </si>
+  <si>
+    <t>bool1</t>
+  </si>
+  <si>
+    <t>bool2</t>
+  </si>
+  <si>
+    <t>bool3</t>
+  </si>
+  <si>
+    <t>bool4</t>
+  </si>
+  <si>
+    <t>bool5</t>
+  </si>
+  <si>
+    <t>=PI()*(Diam_Roll^2 - Diam_Core^2)/(4*Caliper)/1000</t>
   </si>
 </sst>
 </file>
@@ -798,7 +828,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -821,9 +851,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -848,7 +875,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -857,6 +883,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="60% - Accent2" xfId="6" builtinId="36"/>
@@ -1382,23 +1418,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351199EA-EA34-48DB-8F62-7D65D9CC8745}">
-  <dimension ref="A1:K20"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.59765625" customWidth="1"/>
-    <col min="2" max="2" width="7.59765625" customWidth="1"/>
-    <col min="3" max="3" width="17.9296875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.06640625" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="37" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="2" width="2.3984375" customWidth="1"/>
+    <col min="3" max="3" width="22.796875" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" customWidth="1"/>
+    <col min="6" max="6" width="10.796875" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="35.9296875" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="4.59765625" customWidth="1"/>
-    <col min="9" max="9" width="15.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -1408,7 +1444,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1428,31 +1464,31 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C2"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C3"/>
+      <c r="C3" s="40"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="41" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1467,12 +1503,12 @@
       <c r="G5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="32">
         <v>120.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="41" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1487,12 +1523,12 @@
       <c r="G6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="32">
         <v>43.2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="41" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1507,18 +1543,18 @@
       <c r="G7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="33">
         <v>0.47</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1531,32 +1567,32 @@
         <v>35</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="I9" s="10">
-        <f>PI()*($I$5^2-$I$6^2)/(4*$I$7)/1000</f>
+        <f>PI()*(Diam_Roll^2 - Diam_Core^2)/(4*Caliper)/1000</f>
         <v>21.145608965133924</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1571,15 +1607,15 @@
       <c r="G12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="34">
+      <c r="I12" s="32">
         <f>'Raw Data'!P9</f>
         <v>102.2</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="41" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1592,14 +1628,14 @@
       <c r="G13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="35">
         <v>3</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="41" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1614,20 +1650,20 @@
       <c r="G14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="36">
+      <c r="I14" s="34">
         <v>20</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="41" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1640,30 +1676,80 @@
         <v>35</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="I16" s="39">
-        <f>(I12*I13*I14/1000)</f>
+      <c r="I16" s="37">
+        <f>(Length_Unit*n_People*sq_usage/1000)</f>
         <v>6.1319999999999997</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C17" s="8" t="s">
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C17" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C20"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C20" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="32">
+        <v>20</v>
+      </c>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C21" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="38">
+        <f>ROUND(Length_Roll/rate_line,2)</f>
+        <v>1.06</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1674,6 +1760,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE87476B-6205-4D9E-AF8F-2E4CF9937D6A}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -2180,6 +2267,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A35462-56D0-45F7-9764-50AAAA789AD2}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2263,6 +2351,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82288E20-5C2F-4C22-AA69-B647B578D988}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2272,160 +2361,160 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="12.59765625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="20.59765625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="12.59765625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="7.59765625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="12.59765625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="7.59765625" style="24" customWidth="1"/>
-    <col min="9" max="9" width="7.59765625" style="23" customWidth="1"/>
+    <col min="1" max="3" width="12.59765625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="20.59765625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.59765625" style="29" customWidth="1"/>
+    <col min="8" max="8" width="7.59765625" style="23" customWidth="1"/>
+    <col min="9" max="9" width="7.59765625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.45">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="27" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="25"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="27" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="25"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="27" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="25"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="27" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="25"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="27" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="25"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="27" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="25"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="27" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="25"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="27" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="25"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="27" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="25"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2436,4 +2525,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22A016E-2805-4BFB-A886-C373305C40F0}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Roll Length Model TDD/OOP example
</commit_message>
<xml_diff>
--- a/Roll Length Model.xlsx
+++ b/Roll Length Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Practical_Python_For_Modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6066F7-1C9D-4D28-B988-1474FF48D3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A637CE2C-9618-4080-9D1A-BF23ACF1214C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="510" windowWidth="35617" windowHeight="14707" xr2:uid="{4FDF0578-8281-4B11-9B5F-4602E6B37CDC}"/>
+    <workbookView xWindow="1103" yWindow="293" windowWidth="32377" windowHeight="15907" activeTab="1" xr2:uid="{4FDF0578-8281-4B11-9B5F-4602E6B37CDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <definedName name="sq_usage">Model!$I$14</definedName>
     <definedName name="t_run">Model!$I$21</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -244,7 +244,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
   <si>
     <t>Grp</t>
   </si>
@@ -547,13 +547,51 @@
   <si>
     <t>=PI()*(Diam_Roll^2 - Diam_Core^2)/(4*Caliper)/1000</t>
   </si>
+  <si>
+    <t>p/4C</t>
+  </si>
+  <si>
+    <t>pi/(4*slope)</t>
+  </si>
+  <si>
+    <t>1/m</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>diam</t>
+  </si>
+  <si>
+    <t>diam_m</t>
+  </si>
+  <si>
+    <t>diam_m^2</t>
+  </si>
+  <si>
+    <t>0.0000</t>
+  </si>
+  <si>
+    <t>Two-Point test data example 4/27/23</t>
+  </si>
+  <si>
+    <t>from JMP fit</t>
+  </si>
+  <si>
+    <t>caliper</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -828,7 +866,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -878,7 +916,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1"/>
@@ -893,6 +930,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="60% - Accent2" xfId="6" builtinId="36"/>
@@ -1077,7 +1117,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -1421,14 +1461,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="2.3984375" customWidth="1"/>
-    <col min="3" max="3" width="22.796875" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.796875" style="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.19921875" customWidth="1"/>
     <col min="5" max="5" width="11.86328125" customWidth="1"/>
     <col min="6" max="6" width="10.796875" bestFit="1" customWidth="1" outlineLevel="1"/>
@@ -1444,7 +1484,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1464,7 +1504,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C2" s="40"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="5" t="s">
         <v>45</v>
       </c>
@@ -1476,7 +1516,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C3" s="40"/>
+      <c r="C3" s="39"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -1488,7 +1528,7 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="40" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1508,7 +1548,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="40" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1528,7 +1568,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="40" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1538,13 +1578,13 @@
         <v>7</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="33">
-        <v>0.47</v>
+      <c r="I7" s="42">
+        <v>0.50270000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
@@ -1554,7 +1594,7 @@
       <c r="K8" s="18"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="40" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1569,9 +1609,9 @@
       <c r="G9" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="43">
         <f>PI()*(Diam_Roll^2 - Diam_Core^2)/(4*Caliper)/1000</f>
-        <v>21.145608965133924</v>
+        <v>19.770113812637643</v>
       </c>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -1592,7 +1632,7 @@
       <c r="K11" s="18"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1615,7 +1655,7 @@
       <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="40" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1628,14 +1668,14 @@
       <c r="G13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="34">
         <v>3</v>
       </c>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="40" t="s">
         <v>32</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1650,7 +1690,7 @@
       <c r="G14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="33">
         <v>20</v>
       </c>
       <c r="J14" s="18"/>
@@ -1663,7 +1703,7 @@
       <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="40" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1676,7 +1716,7 @@
         <v>35</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="I16" s="37">
+      <c r="I16" s="36">
         <f>(Length_Unit*n_People*sq_usage/1000)</f>
         <v>6.1319999999999997</v>
       </c>
@@ -1684,14 +1724,14 @@
       <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="40" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="30"/>
       <c r="E17" s="30"/>
       <c r="F17" s="31"/>
       <c r="G17" s="31"/>
-      <c r="I17" s="36"/>
+      <c r="I17" s="35"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
     </row>
@@ -1709,7 +1749,7 @@
       <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="40" t="s">
         <v>73</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1731,7 +1771,7 @@
       <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="40" t="s">
         <v>76</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -1746,9 +1786,9 @@
       <c r="G21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="38">
+      <c r="I21" s="37">
         <f>ROUND(Length_Roll/rate_line,2)</f>
-        <v>1.06</v>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>
@@ -1761,14 +1801,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE87476B-6205-4D9E-AF8F-2E4CF9937D6A}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z36" sqref="Z36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.53125" customWidth="1"/>
+    <col min="23" max="23" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.45">
@@ -2242,20 +2286,115 @@
         <v>120.5</v>
       </c>
     </row>
-    <row r="18" spans="22:22" x14ac:dyDescent="0.45">
+    <row r="18" spans="22:28" x14ac:dyDescent="0.45">
       <c r="V18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="22:22" x14ac:dyDescent="0.45">
+    <row r="19" spans="22:28" x14ac:dyDescent="0.45">
       <c r="V19" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="22:22" x14ac:dyDescent="0.45">
+    <row r="20" spans="22:28" x14ac:dyDescent="0.45">
       <c r="V20" t="s">
         <v>70</v>
       </c>
+    </row>
+    <row r="28" spans="22:28" x14ac:dyDescent="0.45">
+      <c r="Y28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="22:28" x14ac:dyDescent="0.45">
+      <c r="Y29" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="22:28" x14ac:dyDescent="0.45">
+      <c r="Y30">
+        <v>20</v>
+      </c>
+      <c r="Z30">
+        <v>120</v>
+      </c>
+      <c r="AA30">
+        <v>0.12</v>
+      </c>
+      <c r="AB30">
+        <f>AA30^2</f>
+        <v>1.44E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="22:28" x14ac:dyDescent="0.45">
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>40</v>
+      </c>
+      <c r="AA31">
+        <v>0.04</v>
+      </c>
+      <c r="AB31">
+        <f>AA31^2</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="25:28" x14ac:dyDescent="0.45">
+      <c r="Z34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="25:28" x14ac:dyDescent="0.45">
+      <c r="Y35" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z35">
+        <v>16349</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="25:28" x14ac:dyDescent="0.45">
+      <c r="Y37" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="25:28" x14ac:dyDescent="0.45">
+      <c r="Z38">
+        <f>PI()/(4*Z35)</f>
+        <v>4.8039523114407503E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="25:28" x14ac:dyDescent="0.45">
+      <c r="Z39">
+        <f>Z38*1000</f>
+        <v>4.8039523114407505E-2</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="25:28" x14ac:dyDescent="0.45">
+      <c r="Y40" s="41"/>
+      <c r="AA40" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>